<commit_message>
2nd version, added "add window"
</commit_message>
<xml_diff>
--- a/expenses/2023.xlsx
+++ b/expenses/2023.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
@@ -900,9 +900,8 @@
     </row>
     <row r="23"/>
     <row r="24"/>
-    <row r="25"/>
-    <row r="26">
-      <c r="B26" s="9" t="n"/>
+    <row r="25">
+      <c r="B25" s="9" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1013,24 +1012,6 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>30/11/2023</t>
-        </is>
-      </c>
-      <c r="B4" s="13" t="n">
-        <v>123</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>fghdf</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>asdfsdf</t>
-        </is>
-      </c>
       <c r="G4" s="7" t="inlineStr">
         <is>
           <t>Montante inicial:</t>
@@ -1041,24 +1022,6 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>30/11/2023</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="n">
-        <v>34</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>saf</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
       <c r="G5" s="7" t="inlineStr">
         <is>
           <t>Montante final:</t>

</xml_diff>

<commit_message>
2nd version - CRUDE operations for expenses and revenues and creating year
</commit_message>
<xml_diff>
--- a/expenses/2023.xlsx
+++ b/expenses/2023.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="360" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,11 +16,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ \€"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00 €"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ \€;[Red]\ \ \-#,##0.00\ \€"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00 €; [Red]-#,##0.00 €"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -64,26 +65,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="40" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -428,13 +422,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="10.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="9" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -467,12 +461,12 @@
           <t>DESCRIPTION</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Data início:</t>
         </is>
       </c>
-      <c r="H1" s="2" t="n">
+      <c r="H1" s="9" t="n">
         <v>45224</v>
       </c>
     </row>
@@ -480,7 +474,7 @@
       <c r="A2" s="2" t="n">
         <v>45224</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="10" t="n">
         <v>11</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -493,12 +487,12 @@
           <t>Carregar o telemóvel</t>
         </is>
       </c>
-      <c r="G2" s="7" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Data fim:</t>
         </is>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="9" t="n">
         <v>45253</v>
       </c>
     </row>
@@ -506,7 +500,7 @@
       <c r="A3" s="2" t="n">
         <v>45224</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="10" t="n">
         <v>89.56999999999999</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -521,10 +515,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45225</v>
-      </c>
-      <c r="B4" s="9" t="n">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>26/10/2023</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="n">
         <v>73.17</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -537,21 +533,20 @@
           <t>Cadeira escritório</t>
         </is>
       </c>
-      <c r="G4" s="7" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Montante inicial:</t>
         </is>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="H4" s="11" t="n">
         <v>959.58</v>
       </c>
-      <c r="I4" s="4" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
         <v>45225</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="10" t="n">
         <v>20.23</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -564,7 +559,7 @@
           <t>Temu - Crocs + Prenda Inês + Aparelho para a aparelhagem</t>
         </is>
       </c>
-      <c r="G5" s="7" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr">
         <is>
           <t>Montante final:</t>
         </is>
@@ -578,7 +573,7 @@
       <c r="A6" s="2" t="n">
         <v>45226</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="10" t="n">
         <v>30</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -596,7 +591,7 @@
       <c r="A7" s="2" t="n">
         <v>45227</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <v>25</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -609,7 +604,7 @@
           <t>Arranjo da corrente da bicla</t>
         </is>
       </c>
-      <c r="G7" s="7" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Total gasto:</t>
         </is>
@@ -623,7 +618,7 @@
       <c r="A8" s="2" t="n">
         <v>45228</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="10" t="n">
         <v>11</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -635,22 +630,13 @@
         <is>
           <t>Saída com os boys (Alex e Dani)</t>
         </is>
-      </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>Total gasto:</t>
-        </is>
-      </c>
-      <c r="H8" s="12">
-        <f>SUM(B:B)</f>
-        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
         <v>45229</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="10" t="n">
         <v>12.74</v>
       </c>
       <c r="C9" t="inlineStr">
@@ -668,7 +654,7 @@
       <c r="A10" s="2" t="n">
         <v>45234</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="10" t="n">
         <v>13.6</v>
       </c>
       <c r="C10" t="inlineStr">
@@ -686,7 +672,7 @@
       <c r="A11" s="2" t="n">
         <v>45236</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B11" s="10" t="n">
         <v>30</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -704,7 +690,7 @@
       <c r="A12" s="2" t="n">
         <v>45238</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="10" t="n">
         <v>12.5</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -722,7 +708,7 @@
       <c r="A13" s="2" t="n">
         <v>45240</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B13" s="10" t="n">
         <v>2.15</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -740,7 +726,7 @@
       <c r="A14" s="2" t="n">
         <v>45241</v>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="10" t="n">
         <v>4.64</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -758,7 +744,7 @@
       <c r="A15" s="2" t="n">
         <v>45241</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="10" t="n">
         <v>1.65</v>
       </c>
       <c r="C15" t="inlineStr">
@@ -776,7 +762,7 @@
       <c r="A16" s="2" t="n">
         <v>45241</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="10" t="n">
         <v>9.1</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -794,7 +780,7 @@
       <c r="A17" s="2" t="n">
         <v>45242</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="10" t="n">
         <v>36.36</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -812,7 +798,7 @@
       <c r="A18" s="2" t="n">
         <v>45244</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="10" t="n">
         <v>5.99</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -830,7 +816,7 @@
       <c r="A19" s="2" t="n">
         <v>45249</v>
       </c>
-      <c r="B19" s="9" t="n">
+      <c r="B19" s="10" t="n">
         <v>50</v>
       </c>
       <c r="C19" t="inlineStr">
@@ -848,7 +834,7 @@
       <c r="A20" s="2" t="n">
         <v>45251</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="10" t="n">
         <v>40</v>
       </c>
       <c r="C20" t="inlineStr">
@@ -866,7 +852,7 @@
       <c r="A21" s="2" t="n">
         <v>45252</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="10" t="n">
         <v>50</v>
       </c>
       <c r="C21" t="inlineStr">
@@ -884,7 +870,7 @@
       <c r="A22" s="2" t="n">
         <v>45252</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>11</v>
       </c>
       <c r="C22" t="inlineStr">
@@ -898,10 +884,8 @@
         </is>
       </c>
     </row>
-    <row r="23"/>
-    <row r="24"/>
     <row r="25">
-      <c r="B25" s="9" t="n"/>
+      <c r="B25" s="10" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -918,13 +902,13 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="10.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
     <col width="17.44140625" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="49.77734375" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="15.33203125" bestFit="1" customWidth="1" min="7" max="7"/>
@@ -939,7 +923,7 @@
           <t>DATE</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>AMOUNT</t>
         </is>
@@ -954,23 +938,25 @@
           <t>DESCRIPTION</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Data início:</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>23/11/2023</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45255</v>
-      </c>
-      <c r="B2" s="9" t="n">
-        <v>7.2</v>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>25/11/2023</t>
+        </is>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>7.3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -982,12 +968,12 @@
           <t>Lanche com Inês - Faro</t>
         </is>
       </c>
-      <c r="G2" s="7" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Data fim:</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>23/12/2023</t>
         </is>
@@ -997,7 +983,7 @@
       <c r="A3" s="2" t="n">
         <v>45257</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="8" t="n">
         <v>59.99</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -1012,7 +998,25 @@
       </c>
     </row>
     <row r="4">
-      <c r="G4" s="7" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>02/01/2024</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Jardim zologico</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>passe</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Montante inicial:</t>
         </is>
@@ -1022,7 +1026,25 @@
       </c>
     </row>
     <row r="5">
-      <c r="G5" s="7" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>04/12/2023</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>-21</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>fgsdfs</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sxvvb</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
         <is>
           <t>Montante final:</t>
         </is>
@@ -1032,9 +1054,8 @@
         <v/>
       </c>
     </row>
-    <row r="6"/>
     <row r="7">
-      <c r="G7" s="7" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Total gasto:</t>
         </is>

</xml_diff>

<commit_message>
3rd version - categories implemented
</commit_message>
<xml_diff>
--- a/expenses/2023.xlsx
+++ b/expenses/2023.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="360" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4296" yWindow="312" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ \€;[Red]\ \ \-#,##0.00\ \€"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ \€;[Red]\ \-#,##0.00\ \€"/>
     <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="168" formatCode="#,##0.00 €; [Red]-#,##0.00 €"/>
   </numFmts>
@@ -72,13 +72,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="40" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,11 +424,11 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="10.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="9" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -461,6 +461,11 @@
           <t>DESCRIPTION</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CATEGORY</t>
+        </is>
+      </c>
       <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Data início:</t>
@@ -487,6 +492,11 @@
           <t>Carregar o telemóvel</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Data fim:</t>
@@ -513,6 +523,11 @@
           <t>Prenda pai (Mi TV Stick) + Relógio Smart Band</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -533,12 +548,17 @@
           <t>Cadeira escritório</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Montante inicial:</t>
         </is>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="12" t="n">
         <v>959.58</v>
       </c>
     </row>
@@ -559,12 +579,17 @@
           <t>Temu - Crocs + Prenda Inês + Aparelho para a aparelhagem</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
           <t>Montante final:</t>
         </is>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="12">
         <f>(H4-H7)</f>
         <v/>
       </c>
@@ -586,6 +611,11 @@
           <t>KapaHemps - Weed</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -604,12 +634,17 @@
           <t>Arranjo da corrente da bicla</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Total gasto:</t>
         </is>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="12">
         <f>SUM(B:B)</f>
         <v/>
       </c>
@@ -631,6 +666,11 @@
           <t>Saída com os boys (Alex e Dani)</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -649,6 +689,11 @@
           <t>Games - Battlefield 1 Premium</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -667,6 +712,11 @@
           <t>Almoço com a Inês</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -685,6 +735,11 @@
           <t>Trading 212 - Disney</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -703,6 +758,11 @@
           <t>Comboio Castro - Lisboa</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -721,6 +781,11 @@
           <t>Cartão + passagem Metro</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -739,6 +804,11 @@
           <t>Uber - Lisboa</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -757,6 +827,11 @@
           <t>Cartão + passagem Metro</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -775,6 +850,11 @@
           <t>Autocarro Lisboa - Castro Verde</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -793,6 +873,11 @@
           <t>Casa para PDA - Sevilha</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -811,6 +896,11 @@
           <t>Uber - Lisboa</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -829,6 +919,11 @@
           <t>Psicóloga</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -847,6 +942,11 @@
           <t>Trading 212 - Intel - 10€ na plataforma</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -865,6 +965,11 @@
           <t>KapaHemps - Weed</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -883,7 +988,14 @@
           <t>Carregar o telemóvel</t>
         </is>
       </c>
-    </row>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
     <row r="25">
       <c r="B25" s="10" t="n"/>
     </row>
@@ -899,18 +1011,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="10.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="9" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
     <col width="17.44140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="49.77734375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="20.33203125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="10.109375" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="15.33203125" bestFit="1" customWidth="1" min="7" max="7"/>
     <col width="10.5546875" bestFit="1" customWidth="1" min="8" max="8"/>
     <col width="10.33203125" bestFit="1" customWidth="1" min="15" max="15"/>
@@ -923,7 +1036,7 @@
           <t>DATE</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>AMOUNT</t>
         </is>
@@ -936,6 +1049,11 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>DESCRIPTION</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CATEGORY</t>
         </is>
       </c>
       <c r="G1" s="4" t="inlineStr">
@@ -955,7 +1073,7 @@
           <t>25/11/2023</t>
         </is>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="7" t="n">
         <v>7.3</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -966,6 +1084,11 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>Lanche com Inês - Faro</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Food</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
@@ -983,7 +1106,7 @@
       <c r="A3" s="2" t="n">
         <v>45257</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="7" t="n">
         <v>59.99</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -994,6 +1117,11 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>Sapatilhas - SportZone</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Food</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1131,7 @@
           <t>02/01/2024</t>
         </is>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="7" t="n">
         <v>1.65</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -1016,12 +1144,17 @@
           <t>passe</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Montante inicial:</t>
         </is>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="12" t="n">
         <v>1400</v>
       </c>
     </row>
@@ -1044,25 +1177,103 @@
           <t>sxvvb</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
           <t>Montante final:</t>
         </is>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="12">
         <f>(H4-H7)</f>
         <v/>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04/12/2023</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>-123</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dfs</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>dfasdf</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>04/12/2023</t>
+        </is>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>231</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>af</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>asdfasd</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Total gasto:</t>
         </is>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="12">
         <f>SUM(B:B)</f>
         <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04/12/2023</t>
+        </is>
+      </c>
+      <c r="B8" s="12" t="n">
+        <v>-12</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sdgdf</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>gsfgbfg</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Health</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3rd version review - addded category "income"
</commit_message>
<xml_diff>
--- a/expenses/2023.xlsx
+++ b/expenses/2023.xlsx
@@ -1011,7 +1011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1223,22 +1223,22 @@
           <t>04/12/2023</t>
         </is>
       </c>
-      <c r="B7" s="11" t="n">
-        <v>231</v>
+      <c r="B7" s="12" t="n">
+        <v>-12</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>af</t>
+          <t>sdgdf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>asdfasd</t>
+          <t>gsfgbfg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Health</t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -1254,25 +1254,50 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>07/12/2023</t>
+        </is>
+      </c>
+      <c r="B8" s="12" t="n">
+        <v>-20</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kdsjfa</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jklsndnvs</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>04/12/2023</t>
         </is>
       </c>
-      <c r="B8" s="12" t="n">
-        <v>-12</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>sdgdf</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>gsfgbfg</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Health</t>
+      <c r="B9" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>pai</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ola</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
5th version - statistics
</commit_message>
<xml_diff>
--- a/expenses/2023.xlsx
+++ b/expenses/2023.xlsx
@@ -510,10 +510,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45224</v>
-      </c>
-      <c r="B3" s="8" t="n">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>25/10/2023</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="n">
         <v>89.56999999999999</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -528,7 +530,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Income</t>
         </is>
       </c>
     </row>
@@ -564,10 +566,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45225</v>
-      </c>
-      <c r="B5" s="8" t="n">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>26/10/2023</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="n">
         <v>20.23</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -582,7 +586,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -893,10 +897,12 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
-        <v>45244</v>
-      </c>
-      <c r="B18" s="8" t="n">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>14/11/2023</t>
+        </is>
+      </c>
+      <c r="B18" s="11" t="n">
         <v>5.99</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -911,7 +917,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Income</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
5th version - bug fixing
</commit_message>
<xml_diff>
--- a/expenses/2023.xlsx
+++ b/expenses/2023.xlsx
@@ -19,9 +19,9 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ \€;[Red]\ \-#,##0.00\ \€"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00 €; [Red]-#,##0.00 €"/>
-    <numFmt numFmtId="168" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00 €; [Red]-#,##0.00 €"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -65,21 +65,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +422,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -472,7 +468,7 @@
           <t>Data início:</t>
         </is>
       </c>
-      <c r="H1" s="10" t="n">
+      <c r="H1" s="6" t="n">
         <v>45224</v>
       </c>
     </row>
@@ -482,7 +478,7 @@
           <t>25/10/2023</t>
         </is>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="7" t="n">
         <v>-89.56999999999999</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -505,7 +501,7 @@
           <t>Data fim:</t>
         </is>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="6" t="n">
         <v>45253</v>
       </c>
     </row>
@@ -515,7 +511,7 @@
           <t>25/10/2023</t>
         </is>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="7" t="n">
         <v>89.56999999999999</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -561,7 +557,7 @@
           <t>Montante inicial:</t>
         </is>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="9" t="n">
         <v>959.58</v>
       </c>
     </row>
@@ -571,7 +567,7 @@
           <t>26/10/2023</t>
         </is>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="7" t="n">
         <v>20.23</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -594,7 +590,7 @@
           <t>Montante final:</t>
         </is>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <f>(H4-H7)</f>
         <v/>
       </c>
@@ -628,7 +624,7 @@
           <t>29/10/2023</t>
         </is>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="7" t="n">
         <v>-11</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -651,7 +647,7 @@
           <t>Total gasto:</t>
         </is>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <f>SUM(B:B)</f>
         <v/>
       </c>
@@ -662,7 +658,7 @@
           <t>30/10/2023</t>
         </is>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="7" t="n">
         <v>-12.74</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -733,7 +729,7 @@
           <t>08/11/2023</t>
         </is>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="7" t="n">
         <v>-12.5</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -804,7 +800,7 @@
           <t>11/11/2023</t>
         </is>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="7" t="n">
         <v>-1.65</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -852,7 +848,7 @@
           <t>12/11/2023</t>
         </is>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="7" t="n">
         <v>-36.36</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -877,7 +873,7 @@
           <t>14/11/2023</t>
         </is>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="7" t="n">
         <v>-5.99</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -902,7 +898,7 @@
           <t>14/11/2023</t>
         </is>
       </c>
-      <c r="B18" s="11" t="n">
+      <c r="B18" s="7" t="n">
         <v>5.99</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -1031,10 +1027,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -1080,32 +1076,32 @@
           <t>Data início:</t>
         </is>
       </c>
-      <c r="H1" s="10" t="n">
+      <c r="H1" s="6" t="n">
         <v>45253</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>27/11/2023</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="n">
-        <v>-59.99</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>13/12/2023</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>-1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HIPAY SAS</t>
+          <t>a</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sapatilhas - SportZone</t>
+          <t>a</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Education</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
@@ -1113,142 +1109,66 @@
           <t>Data fim:</t>
         </is>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="6" t="n">
         <v>45283</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>27/11/2023</t>
-        </is>
-      </c>
-      <c r="B3" s="11" t="n">
-        <v>-59.99</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>HIPAY SAS</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Sapatilhas - SportZone</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-    </row>
+    <row r="3"/>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
-      <c r="B4" s="8" t="n"/>
+      <c r="B4" s="7" t="n"/>
       <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Montante inicial:</t>
         </is>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="9" t="n">
         <v>1407.14</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
-      <c r="B5" s="8" t="n"/>
       <c r="G5" s="4" t="inlineStr">
         <is>
           <t>Montante final:</t>
         </is>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <f>(H4-H7)</f>
         <v/>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="n"/>
-      <c r="B6" s="8" t="n"/>
-    </row>
+    <row r="6"/>
     <row r="7">
-      <c r="A7" s="2" t="n"/>
-      <c r="B7" s="8" t="n"/>
       <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Total gasto:</t>
         </is>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <f>SUM(B:B)</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n"/>
-      <c r="B8" s="8" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n"/>
-      <c r="B9" s="8" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="8" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n"/>
-      <c r="B11" s="8" t="n"/>
-    </row>
+      <c r="B8" s="7" t="n"/>
+    </row>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12">
-      <c r="A12" s="2" t="n"/>
-      <c r="B12" s="8" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n"/>
-      <c r="B13" s="8" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n"/>
-      <c r="B14" s="8" t="n"/>
-    </row>
+      <c r="B12" s="7" t="n"/>
+    </row>
+    <row r="13"/>
+    <row r="14"/>
     <row r="15">
-      <c r="A15" s="2" t="n"/>
-      <c r="B15" s="8" t="n"/>
+      <c r="B15" s="7" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n"/>
-      <c r="B16" s="8" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n"/>
-      <c r="B17" s="8" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n"/>
-      <c r="B18" s="8" t="n"/>
-    </row>
+      <c r="B16" s="7" t="n"/>
+    </row>
+    <row r="17"/>
+    <row r="18"/>
     <row r="19">
-      <c r="A19" s="2" t="n"/>
-      <c r="B19" s="8" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n"/>
-      <c r="B20" s="8" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n"/>
-      <c r="B21" s="8" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n"/>
-      <c r="B22" s="8" t="n"/>
-    </row>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26">
-      <c r="B26" s="8" t="n"/>
+      <c r="B19" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>